<commit_message>
update Team and Course table structure and add a new team and complete course details and update mate table
</commit_message>
<xml_diff>
--- a/src/DB.xlsx
+++ b/src/DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jisasg8\Documents\Study\Java\Quiz_Portal_WebService\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FA2CCA-8FF4-4CF0-8B46-42172BD12D94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EF0B54-4762-47E1-AC7F-D88B70DAC67A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F3B72F42-65FD-493E-8AC5-CF0DB73918A9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{F3B72F42-65FD-493E-8AC5-CF0DB73918A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="64">
   <si>
     <t>MCQ</t>
   </si>
@@ -128,9 +128,6 @@
     <t>TeamID</t>
   </si>
   <si>
-    <t>TeamName</t>
-  </si>
-  <si>
     <t>CreatedBy</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
     <t>CourseID</t>
   </si>
   <si>
-    <t>CourseName</t>
-  </si>
-  <si>
     <t>QuestionID</t>
   </si>
   <si>
@@ -201,6 +195,39 @@
   </si>
   <si>
     <t>Simon Now</t>
+  </si>
+  <si>
+    <t>NumberOfQuestions</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>https://www.truck-n-trailer.com/wp-content/uploads/TrucknTrailer_Blog1-010919.jpg</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>It is a long established fact that a reader will be distracted by the readable content of a page when looking at its layout. The point of using Lorem Ipsum is that it has a more-or-less normal distribution of letters, as opposed to using 'Content here, content here', making it look like readable English. Many desktop publishing packages and web page editors now use Lorem Ipsum as their default model text, and a search for 'lorem ipsum' will uncover many web sites still in their infancy. Various versions have evolved over the years, sometimes by accident, sometimes on purpose (injected humour and the like).</t>
+  </si>
+  <si>
+    <t>Lorem Ipsum is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an unknown printer took a galley of type and scrambled it to make a type specimen book. It has survived not only five centuries, but also the leap into electronic typesetting, remaining essentially unchanged. It was popularised in the 1960s with the release of Letraset sheets containing Lorem Ipsum passages, and more recently with desktop publishing software like Aldus PageMaker including versions of Lorem Ipsum.</t>
+  </si>
+  <si>
+    <t>There are many variations of passages of Lorem Ipsum available, but the majority have suffered alteration in some form, by injected humour, or randomised words which don't look even slightly believable. If you are going to use a passage of Lorem Ipsum, you need to be sure there isn't anything embarrassing hidden in the middle of text. All the Lorem Ipsum generators on the Internet tend to repeat predefined chunks as necessary,</t>
+  </si>
+  <si>
+    <t>The standard chunk of Lorem Ipsum used since the 1500s is reproduced below for those interested. Sections 1.10.32 and 1.10.33 from "de Finibus Bonorum et Malorum" by Cicero are also reproduced in their exact original form, accompanied by English versions from the 1914 translation by H. Rackham.</t>
+  </si>
+  <si>
+    <t>DurationInMins</t>
   </si>
 </sst>
 </file>
@@ -561,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961BB5A6-B99A-4A1C-AA0A-519641453626}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -583,7 +610,7 @@
         <v>26</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -609,29 +636,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428C1560-C610-4E19-8B16-17E25FF4640B}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -639,7 +669,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -648,7 +678,7 @@
         <v>43990</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -656,7 +686,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -665,7 +695,24 @@
         <v>43991</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44005</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -676,71 +723,156 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8FE03B-A7B0-4C40-9357-E3EF31DD116D}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1796875" customWidth="1"/>
+    <col min="7" max="7" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1">
+        <v>44005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1">
+        <v>44005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1">
+        <v>44005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1">
+        <v>44005</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -762,52 +894,52 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>37</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>38</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>39</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>40</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>41</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>42</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>43</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>44</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>45</v>
       </c>
-      <c r="M1" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" t="s">
-        <v>47</v>
-      </c>
       <c r="O1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" t="s">
         <v>31</v>
-      </c>
-      <c r="P1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
remove console messages and display full error messages on console
</commit_message>
<xml_diff>
--- a/src/DB.xlsx
+++ b/src/DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jisasg8\Documents\Study\Java\Quiz_Portal_WebService\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79958CC-81CB-4FEE-86A5-336F2BF7516C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0DC867-94D2-4138-AAC8-4732A346EC98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{F3B72F42-65FD-493E-8AC5-CF0DB73918A9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
   <si>
     <t>MCQ</t>
   </si>
@@ -53,18 +53,6 @@
     <t>RBI</t>
   </si>
   <si>
-    <t>cat</t>
-  </si>
-  <si>
-    <t>dog</t>
-  </si>
-  <si>
-    <t>tiger</t>
-  </si>
-  <si>
-    <t>lion</t>
-  </si>
-  <si>
     <t>elephant</t>
   </si>
   <si>
@@ -222,6 +210,57 @@
   </si>
   <si>
     <t>fkhsdf</t>
+  </si>
+  <si>
+    <t>DDD stands for?</t>
+  </si>
+  <si>
+    <t>ACB</t>
+  </si>
+  <si>
+    <t>HEF</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>You</t>
+  </si>
+  <si>
+    <t>SME</t>
+  </si>
+  <si>
+    <t>Who can have a alpha?</t>
+  </si>
+  <si>
+    <t>Backoffice</t>
+  </si>
+  <si>
+    <t>Operations</t>
+  </si>
+  <si>
+    <t>Which offshore team handle issue related a driver?</t>
+  </si>
+  <si>
+    <t>How are all SMEs for Vehicle?</t>
+  </si>
+  <si>
+    <t>Jamie</t>
+  </si>
+  <si>
+    <t>Anitha</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Vlad</t>
+  </si>
+  <si>
+    <t>Prasanna</t>
   </si>
 </sst>
 </file>
@@ -593,15 +632,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -609,7 +648,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -617,7 +656,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -643,19 +682,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -663,7 +702,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -672,7 +711,7 @@
         <v>43990</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -680,7 +719,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -689,7 +728,7 @@
         <v>43991</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -697,7 +736,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -706,7 +745,7 @@
         <v>44005</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -736,28 +775,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -768,10 +807,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -794,10 +833,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -823,7 +862,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -846,10 +885,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -875,7 +914,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -889,52 +928,52 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>33</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" t="s">
-        <v>38</v>
-      </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="P1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
@@ -945,25 +984,25 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -983,31 +1022,31 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -1027,25 +1066,22 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -1054,12 +1090,9 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
         <v>0</v>
       </c>
       <c r="O4" t="s">
@@ -1077,40 +1110,40 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5" t="s">
         <v>2</v>
@@ -1127,25 +1160,25 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
       </c>
       <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
         <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -1177,25 +1210,25 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" t="s">
         <v>14</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" t="s">
-        <v>18</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -1227,25 +1260,25 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
         <v>14</v>
-      </c>
-      <c r="F8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" t="s">
-        <v>18</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1277,25 +1310,25 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
         <v>14</v>
-      </c>
-      <c r="F9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" t="s">
-        <v>18</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -1327,22 +1360,22 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
         <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" t="s">
-        <v>17</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1371,16 +1404,16 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J11">
         <v>1</v>

</xml_diff>

<commit_message>
add more courses and questions in DB
</commit_message>
<xml_diff>
--- a/src/DB.xlsx
+++ b/src/DB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jisasg8\Documents\Study\Java\Quiz_Portal_WebService\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jisasg8\Downloads\Java\Quiz_Portal_WebService\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0DC867-94D2-4138-AAC8-4732A346EC98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2407E6-4083-47DB-AF75-44D79A36F44E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{F3B72F42-65FD-493E-8AC5-CF0DB73918A9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="209">
   <si>
     <t>MCQ</t>
   </si>
@@ -47,42 +47,9 @@
     <t>Subhendu</t>
   </si>
   <si>
-    <t>Sudhakar</t>
-  </si>
-  <si>
     <t>RBI</t>
   </si>
   <si>
-    <t>elephant</t>
-  </si>
-  <si>
-    <t>ant</t>
-  </si>
-  <si>
-    <t>zebra</t>
-  </si>
-  <si>
-    <t>girref</t>
-  </si>
-  <si>
-    <t>rat</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
     <t>DDD</t>
   </si>
   <si>
@@ -158,9 +125,6 @@
     <t>https://encrypted-tbn0.gstatic.com/images?q=tbn%3AANd9GcTREt3mX0ltMwSWflmD7WntcsMTlWKtqfgEth8rfOOwjsNboutd&amp;usqp=CAU</t>
   </si>
   <si>
-    <t>Safety Training</t>
-  </si>
-  <si>
     <t>Simon Now</t>
   </si>
   <si>
@@ -203,15 +167,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>kcvksdf</t>
-  </si>
-  <si>
-    <t>dkjfh</t>
-  </si>
-  <si>
-    <t>fkhsdf</t>
-  </si>
-  <si>
     <t>DDD stands for?</t>
   </si>
   <si>
@@ -261,6 +216,453 @@
   </si>
   <si>
     <t>Prasanna</t>
+  </si>
+  <si>
+    <t>What is the DB for Safety?</t>
+  </si>
+  <si>
+    <t>Safety_PRD</t>
+  </si>
+  <si>
+    <t>SafetyPRD</t>
+  </si>
+  <si>
+    <t>Safety_PROD</t>
+  </si>
+  <si>
+    <t>SafetyPROD</t>
+  </si>
+  <si>
+    <t>SFTPRD</t>
+  </si>
+  <si>
+    <t>Who can approve a review pending with Safety Manager?</t>
+  </si>
+  <si>
+    <t>Operation Manager</t>
+  </si>
+  <si>
+    <t>Area Risk Manager</t>
+  </si>
+  <si>
+    <t>Fleet Manager</t>
+  </si>
+  <si>
+    <t>Transportation Manager</t>
+  </si>
+  <si>
+    <t>Safety Regional Manager</t>
+  </si>
+  <si>
+    <t>A review can be completed/send to driver when the Training is in assigned status itself?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Reviews will be created for both preventable and non preventable incidents</t>
+  </si>
+  <si>
+    <t>Who can force close a review?</t>
+  </si>
+  <si>
+    <t>Safety Director</t>
+  </si>
+  <si>
+    <t>Safety Manager</t>
+  </si>
+  <si>
+    <t>Manager Hierarchy 1</t>
+  </si>
+  <si>
+    <t>Manager Hierarchy 2</t>
+  </si>
+  <si>
+    <t>Financial and Nonfinancial are the two types of awards</t>
+  </si>
+  <si>
+    <t>What is the workflow for Award processing</t>
+  </si>
+  <si>
+    <t>Processed,Nominated, Approved</t>
+  </si>
+  <si>
+    <t>Nominated, Approved, Processed</t>
+  </si>
+  <si>
+    <t>Approved, Processed, Nominated</t>
+  </si>
+  <si>
+    <t>Processed, Approved, Nominated</t>
+  </si>
+  <si>
+    <t>Any of the above depending on the award type</t>
+  </si>
+  <si>
+    <t>Briefing is created for?</t>
+  </si>
+  <si>
+    <t>For all shipments</t>
+  </si>
+  <si>
+    <t>Both A and B</t>
+  </si>
+  <si>
+    <t>Briefing can be done for bogus driver</t>
+  </si>
+  <si>
+    <t>What is the mode of training assigned to the Particular fleet of drivers?</t>
+  </si>
+  <si>
+    <t>BU level assignement</t>
+  </si>
+  <si>
+    <t>Employee level Assignment</t>
+  </si>
+  <si>
+    <t>Board level Assignment</t>
+  </si>
+  <si>
+    <t>Fleet level assignment</t>
+  </si>
+  <si>
+    <t>All of the above</t>
+  </si>
+  <si>
+    <t>Modules with previleges as "All" can assigned by Safety admins?</t>
+  </si>
+  <si>
+    <t>Which of the following is a CVE event?</t>
+  </si>
+  <si>
+    <t>Collision Mitigation</t>
+  </si>
+  <si>
+    <t>Roll stability</t>
+  </si>
+  <si>
+    <t>Excessive breaking</t>
+  </si>
+  <si>
+    <t>Head way</t>
+  </si>
+  <si>
+    <t>Award</t>
+  </si>
+  <si>
+    <t>Briefing</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>CVE</t>
+  </si>
+  <si>
+    <t>Manimala</t>
+  </si>
+  <si>
+    <t>DDD stands for ?</t>
+  </si>
+  <si>
+    <t>Driver Document Database</t>
+  </si>
+  <si>
+    <t>Driver  Database Documents</t>
+  </si>
+  <si>
+    <t>Database for Driver Document</t>
+  </si>
+  <si>
+    <t>Which offshore team handle issue related a driver review?</t>
+  </si>
+  <si>
+    <t>If a ticket raised by the driver, to whom you should reachout first</t>
+  </si>
+  <si>
+    <t>Driver's Manager</t>
+  </si>
+  <si>
+    <t>Helpdesk</t>
+  </si>
+  <si>
+    <t>Driver's ARM</t>
+  </si>
+  <si>
+    <t>What are all onboard reviews from the following</t>
+  </si>
+  <si>
+    <t>1 Day</t>
+  </si>
+  <si>
+    <t>Collision</t>
+  </si>
+  <si>
+    <t>180 Days</t>
+  </si>
+  <si>
+    <t>60 Days</t>
+  </si>
+  <si>
+    <t>Annual</t>
+  </si>
+  <si>
+    <t>What are all event reviews from the following</t>
+  </si>
+  <si>
+    <t>Seatbelt Citation</t>
+  </si>
+  <si>
+    <t>Incident</t>
+  </si>
+  <si>
+    <t>DOT Inspection</t>
+  </si>
+  <si>
+    <t>For a CVE Headway review creation, at least how many Headway events requierd</t>
+  </si>
+  <si>
+    <t>DOT Inspection, Incident, Collision, etc.. Events reports by</t>
+  </si>
+  <si>
+    <t>Safety Direct</t>
+  </si>
+  <si>
+    <t>PeopleNet</t>
+  </si>
+  <si>
+    <t>Stars</t>
+  </si>
+  <si>
+    <t>What is the Database for DDD</t>
+  </si>
+  <si>
+    <t>SafetySpringBatch_PRD</t>
+  </si>
+  <si>
+    <t>SafetyDriverReview_PRD</t>
+  </si>
+  <si>
+    <t>Stars_PRD</t>
+  </si>
+  <si>
+    <t>What is the Database for Awards</t>
+  </si>
+  <si>
+    <t>Awards has been provied to the</t>
+  </si>
+  <si>
+    <t>Drivers</t>
+  </si>
+  <si>
+    <t>Drivers' Managers</t>
+  </si>
+  <si>
+    <t>ARMs</t>
+  </si>
+  <si>
+    <t>IT Support teams</t>
+  </si>
+  <si>
+    <t>How is Safet Awards are available</t>
+  </si>
+  <si>
+    <t>S1 to S20</t>
+  </si>
+  <si>
+    <t>S1 to S40</t>
+  </si>
+  <si>
+    <t>S1 - Infinity</t>
+  </si>
+  <si>
+    <t>Only S1</t>
+  </si>
+  <si>
+    <t>We can calculate the actual miles for a time periods of currect Year from which Database</t>
+  </si>
+  <si>
+    <t>BIPS</t>
+  </si>
+  <si>
+    <t>DB2P</t>
+  </si>
+  <si>
+    <t>We can calculate the actual miles for a time periods of previous Years from which Database</t>
+  </si>
+  <si>
+    <t>If a Local driver has not driven more then 21 days continuously, then his award/penalty miles should be</t>
+  </si>
+  <si>
+    <t>274*number of days he driven</t>
+  </si>
+  <si>
+    <t>274*number of days in the month</t>
+  </si>
+  <si>
+    <t>As same as his actual miles but not more than 493*number of days in the month</t>
+  </si>
+  <si>
+    <t>If a Local driver has not driven leass then 21 days continuously, then his award/penalty miles should be</t>
+  </si>
+  <si>
+    <t>For a Regional or OTR driver award/penalty miles should be</t>
+  </si>
+  <si>
+    <t>CVE Stands for?</t>
+  </si>
+  <si>
+    <t>Critical Vehicle Events</t>
+  </si>
+  <si>
+    <t>Commom Vehicle Events</t>
+  </si>
+  <si>
+    <t>Critical Valuable Events</t>
+  </si>
+  <si>
+    <t>Critical Vehicle Environment</t>
+  </si>
+  <si>
+    <t>CVE events provides are</t>
+  </si>
+  <si>
+    <t>How can access training portal</t>
+  </si>
+  <si>
+    <t>All JBHunt Employees</t>
+  </si>
+  <si>
+    <t>Only Drivers</t>
+  </si>
+  <si>
+    <t>Only Driver's Managers</t>
+  </si>
+  <si>
+    <t>Who can create new courses</t>
+  </si>
+  <si>
+    <t>Training Admin</t>
+  </si>
+  <si>
+    <t>Anyone</t>
+  </si>
+  <si>
+    <t>How much time takes to reflect result in Training Analytics</t>
+  </si>
+  <si>
+    <t>Immediately</t>
+  </si>
+  <si>
+    <t>1 Hour</t>
+  </si>
+  <si>
+    <t>12 Hours</t>
+  </si>
+  <si>
+    <t>Overnight</t>
+  </si>
+  <si>
+    <t>How many segments should have in a training module</t>
+  </si>
+  <si>
+    <t>At least One</t>
+  </si>
+  <si>
+    <t>No at all</t>
+  </si>
+  <si>
+    <t>Only One</t>
+  </si>
+  <si>
+    <t>What is the Database for Training</t>
+  </si>
+  <si>
+    <t>A course can be assigned to a driver via</t>
+  </si>
+  <si>
+    <t>Training Portal</t>
+  </si>
+  <si>
+    <t>Associatiating with Review from DDD</t>
+  </si>
+  <si>
+    <t>Safety Award App</t>
+  </si>
+  <si>
+    <t>CVE Platform</t>
+  </si>
+  <si>
+    <t>What is the duration for penalty period for the driver?</t>
+  </si>
+  <si>
+    <t>1 Year</t>
+  </si>
+  <si>
+    <t>I month</t>
+  </si>
+  <si>
+    <t>6 months</t>
+  </si>
+  <si>
+    <t>1 week</t>
+  </si>
+  <si>
+    <t>10 months</t>
+  </si>
+  <si>
+    <t>For which incident, the penalty period is calculated for driver?</t>
+  </si>
+  <si>
+    <t>Preventable incident</t>
+  </si>
+  <si>
+    <t>Non preventable incident</t>
+  </si>
+  <si>
+    <t>Can a driver assign the training to himself?</t>
+  </si>
+  <si>
+    <t>Who can assign the training to driver?</t>
+  </si>
+  <si>
+    <t>Two</t>
+  </si>
+  <si>
+    <t>Three</t>
+  </si>
+  <si>
+    <t>Four</t>
+  </si>
+  <si>
+    <t>Five</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>To whom a training can be assigned?</t>
+  </si>
+  <si>
+    <t>Driver himself</t>
+  </si>
+  <si>
+    <t>IT Support team</t>
+  </si>
+  <si>
+    <t>Shivasri</t>
+  </si>
+  <si>
+    <t>A) Transporting High value materials</t>
+  </si>
+  <si>
+    <t>B) Transporting Hazardous Material</t>
+  </si>
+  <si>
+    <t>C) Transporting Chemical Materials</t>
   </si>
 </sst>
 </file>
@@ -622,7 +1024,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -632,15 +1034,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -648,18 +1050,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -682,19 +1084,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -702,7 +1104,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -711,7 +1113,7 @@
         <v>43990</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -719,7 +1121,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -728,7 +1130,7 @@
         <v>43991</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -736,7 +1138,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -745,7 +1147,7 @@
         <v>44005</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -756,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8FE03B-A7B0-4C40-9357-E3EF31DD116D}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -775,28 +1177,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -807,10 +1209,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -833,10 +1235,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>106</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -859,10 +1261,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -885,10 +1287,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -901,6 +1303,84 @@
       </c>
       <c r="H5" s="1">
         <v>44005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="1">
+        <v>44055</v>
       </c>
     </row>
   </sheetData>
@@ -911,10 +1391,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB1996B-3142-4866-82E9-2BEEAEB81BA3}">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -928,52 +1408,52 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="H1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="I1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="J1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="K1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="L1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="M1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="N1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="O1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="P1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
@@ -984,19 +1464,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -1022,22 +1502,22 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="H3" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -1066,22 +1546,22 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -1110,25 +1590,25 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="H5" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="I5" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -1157,28 +1637,28 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="I6" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -1196,10 +1676,10 @@
         <v>0</v>
       </c>
       <c r="O6" t="s">
-        <v>2</v>
+        <v>108</v>
       </c>
       <c r="P6" s="1">
-        <v>44019</v>
+        <v>44055</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
@@ -1207,28 +1687,28 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -1246,10 +1726,10 @@
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>2</v>
+        <v>108</v>
       </c>
       <c r="P7" s="1">
-        <v>44020</v>
+        <v>44055</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
@@ -1257,49 +1737,31 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8" t="s">
-        <v>2</v>
+        <v>108</v>
       </c>
       <c r="P8" s="1">
-        <v>44021</v>
+        <v>44055</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
@@ -1307,49 +1769,31 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="P9" s="1">
-        <v>44022</v>
+        <v>44055</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
@@ -1357,43 +1801,49 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="H10" t="s">
-        <v>13</v>
+        <v>79</v>
+      </c>
+      <c r="I10" t="s">
+        <v>80</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
       </c>
       <c r="O10" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="P10" s="1">
-        <v>44023</v>
+        <v>44055</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
@@ -1401,31 +1851,1623 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="O11" t="s">
+        <v>108</v>
+      </c>
+      <c r="P11" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" t="s">
+        <v>87</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12" t="s">
+        <v>108</v>
+      </c>
+      <c r="P12" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>206</v>
+      </c>
+      <c r="F13" t="s">
+        <v>207</v>
+      </c>
+      <c r="G13" t="s">
+        <v>208</v>
+      </c>
+      <c r="H13" t="s">
+        <v>89</v>
+      </c>
+      <c r="I13" t="s">
+        <v>90</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13" t="s">
+        <v>108</v>
+      </c>
+      <c r="P13" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" t="s">
+        <v>74</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="O14" t="s">
+        <v>108</v>
+      </c>
+      <c r="P14" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" t="s">
+        <v>96</v>
+      </c>
+      <c r="I15" t="s">
+        <v>97</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15" t="s">
+        <v>108</v>
+      </c>
+      <c r="P15" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" t="s">
+        <v>74</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
+        <v>108</v>
+      </c>
+      <c r="P16" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17" t="s">
+        <v>102</v>
+      </c>
+      <c r="H17" t="s">
+        <v>103</v>
+      </c>
+      <c r="I17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17" t="s">
+        <v>108</v>
+      </c>
+      <c r="P17" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" t="s">
+        <v>111</v>
+      </c>
+      <c r="G18" t="s">
+        <v>112</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
+        <v>2</v>
+      </c>
+      <c r="P18" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
+        <v>2</v>
+      </c>
+      <c r="P19" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" t="s">
+        <v>52</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="O20" t="s">
+        <v>2</v>
+      </c>
+      <c r="P20" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
         <v>55</v>
       </c>
-      <c r="D11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F21" t="s">
         <v>56</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G21" t="s">
         <v>57</v>
       </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="O11" t="s">
-        <v>2</v>
-      </c>
-      <c r="P11" s="1">
-        <v>44014</v>
+      <c r="H21" t="s">
+        <v>58</v>
+      </c>
+      <c r="I21" t="s">
+        <v>59</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21" t="s">
+        <v>2</v>
+      </c>
+      <c r="P21" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" t="s">
+        <v>115</v>
+      </c>
+      <c r="G22" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" t="s">
+        <v>116</v>
+      </c>
+      <c r="I22" t="s">
+        <v>117</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22" t="s">
+        <v>2</v>
+      </c>
+      <c r="P22" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" t="s">
+        <v>121</v>
+      </c>
+      <c r="H23" t="s">
+        <v>122</v>
+      </c>
+      <c r="I23" t="s">
+        <v>123</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23" t="s">
+        <v>2</v>
+      </c>
+      <c r="P23" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>125</v>
+      </c>
+      <c r="F24" t="s">
+        <v>120</v>
+      </c>
+      <c r="G24" t="s">
+        <v>126</v>
+      </c>
+      <c r="H24" t="s">
+        <v>123</v>
+      </c>
+      <c r="I24" t="s">
+        <v>127</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24" t="s">
+        <v>2</v>
+      </c>
+      <c r="P24" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>197</v>
+      </c>
+      <c r="F25" t="s">
+        <v>198</v>
+      </c>
+      <c r="G25" t="s">
+        <v>199</v>
+      </c>
+      <c r="H25" t="s">
+        <v>200</v>
+      </c>
+      <c r="I25" t="s">
+        <v>201</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25" t="s">
+        <v>2</v>
+      </c>
+      <c r="P25" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>130</v>
+      </c>
+      <c r="F26" t="s">
+        <v>131</v>
+      </c>
+      <c r="G26" t="s">
+        <v>132</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="O26" t="s">
+        <v>2</v>
+      </c>
+      <c r="P26" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>133</v>
+      </c>
+      <c r="D27" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" t="s">
+        <v>134</v>
+      </c>
+      <c r="G27" t="s">
+        <v>135</v>
+      </c>
+      <c r="H27" t="s">
+        <v>136</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="O27" t="s">
+        <v>2</v>
+      </c>
+      <c r="P27" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>137</v>
+      </c>
+      <c r="D28" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" t="s">
+        <v>134</v>
+      </c>
+      <c r="G28" t="s">
+        <v>135</v>
+      </c>
+      <c r="H28" t="s">
+        <v>136</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="O28" t="s">
+        <v>2</v>
+      </c>
+      <c r="P28" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>138</v>
+      </c>
+      <c r="D29" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>139</v>
+      </c>
+      <c r="F29" t="s">
+        <v>140</v>
+      </c>
+      <c r="G29" t="s">
+        <v>141</v>
+      </c>
+      <c r="H29" t="s">
+        <v>142</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="O29" t="s">
+        <v>2</v>
+      </c>
+      <c r="P29" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>144</v>
+      </c>
+      <c r="F30" t="s">
+        <v>145</v>
+      </c>
+      <c r="G30" t="s">
+        <v>146</v>
+      </c>
+      <c r="H30" t="s">
+        <v>147</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="O30" t="s">
+        <v>2</v>
+      </c>
+      <c r="P30" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>148</v>
+      </c>
+      <c r="D31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>135</v>
+      </c>
+      <c r="F31" t="s">
+        <v>149</v>
+      </c>
+      <c r="G31" t="s">
+        <v>150</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="O31" t="s">
+        <v>2</v>
+      </c>
+      <c r="P31" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>151</v>
+      </c>
+      <c r="D32" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>135</v>
+      </c>
+      <c r="F32" t="s">
+        <v>149</v>
+      </c>
+      <c r="G32" t="s">
+        <v>150</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="O32" t="s">
+        <v>2</v>
+      </c>
+      <c r="P32" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>152</v>
+      </c>
+      <c r="D33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>153</v>
+      </c>
+      <c r="F33" t="s">
+        <v>154</v>
+      </c>
+      <c r="G33" t="s">
+        <v>155</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="O33" t="s">
+        <v>2</v>
+      </c>
+      <c r="P33" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>153</v>
+      </c>
+      <c r="F34" t="s">
+        <v>154</v>
+      </c>
+      <c r="G34" t="s">
+        <v>155</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="O34" t="s">
+        <v>2</v>
+      </c>
+      <c r="P34" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>153</v>
+      </c>
+      <c r="F35" t="s">
+        <v>154</v>
+      </c>
+      <c r="G35" t="s">
+        <v>155</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="O35" t="s">
+        <v>2</v>
+      </c>
+      <c r="P35" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>158</v>
+      </c>
+      <c r="D36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>159</v>
+      </c>
+      <c r="F36" t="s">
+        <v>160</v>
+      </c>
+      <c r="G36" t="s">
+        <v>161</v>
+      </c>
+      <c r="H36" t="s">
+        <v>162</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="O36" t="s">
+        <v>2</v>
+      </c>
+      <c r="P36" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>163</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>130</v>
+      </c>
+      <c r="F37" t="s">
+        <v>131</v>
+      </c>
+      <c r="G37" t="s">
+        <v>132</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="O37" t="s">
+        <v>2</v>
+      </c>
+      <c r="P37" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>164</v>
+      </c>
+      <c r="D38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>165</v>
+      </c>
+      <c r="F38" t="s">
+        <v>166</v>
+      </c>
+      <c r="G38" t="s">
+        <v>167</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="O38" t="s">
+        <v>2</v>
+      </c>
+      <c r="P38" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>168</v>
+      </c>
+      <c r="D39" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>169</v>
+      </c>
+      <c r="F39" t="s">
+        <v>170</v>
+      </c>
+      <c r="G39" t="s">
+        <v>47</v>
+      </c>
+      <c r="H39" t="s">
+        <v>115</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="O39" t="s">
+        <v>2</v>
+      </c>
+      <c r="P39" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>171</v>
+      </c>
+      <c r="D40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F40" t="s">
+        <v>173</v>
+      </c>
+      <c r="G40" t="s">
+        <v>174</v>
+      </c>
+      <c r="H40" t="s">
+        <v>175</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="O40" t="s">
+        <v>2</v>
+      </c>
+      <c r="P40" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>176</v>
+      </c>
+      <c r="D41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>177</v>
+      </c>
+      <c r="F41" t="s">
+        <v>178</v>
+      </c>
+      <c r="G41" t="s">
+        <v>179</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="O41" t="s">
+        <v>2</v>
+      </c>
+      <c r="P41" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>180</v>
+      </c>
+      <c r="D42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" t="s">
+        <v>134</v>
+      </c>
+      <c r="G42" t="s">
+        <v>135</v>
+      </c>
+      <c r="H42" t="s">
+        <v>136</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="O42" t="s">
+        <v>2</v>
+      </c>
+      <c r="P42" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>181</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>182</v>
+      </c>
+      <c r="F43" t="s">
+        <v>183</v>
+      </c>
+      <c r="G43" t="s">
+        <v>184</v>
+      </c>
+      <c r="H43" t="s">
+        <v>185</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="O43" t="s">
+        <v>2</v>
+      </c>
+      <c r="P43" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>186</v>
+      </c>
+      <c r="D44" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" t="s">
+        <v>187</v>
+      </c>
+      <c r="F44" t="s">
+        <v>188</v>
+      </c>
+      <c r="G44" t="s">
+        <v>189</v>
+      </c>
+      <c r="H44" t="s">
+        <v>190</v>
+      </c>
+      <c r="I44" t="s">
+        <v>191</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44" t="s">
+        <v>205</v>
+      </c>
+      <c r="P44" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>192</v>
+      </c>
+      <c r="D45" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" t="s">
+        <v>193</v>
+      </c>
+      <c r="F45" t="s">
+        <v>194</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="O45" t="s">
+        <v>205</v>
+      </c>
+      <c r="P45" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>202</v>
+      </c>
+      <c r="D46" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" t="s">
+        <v>46</v>
+      </c>
+      <c r="F46" t="s">
+        <v>47</v>
+      </c>
+      <c r="G46" t="s">
+        <v>48</v>
+      </c>
+      <c r="H46" t="s">
+        <v>49</v>
+      </c>
+      <c r="I46" t="s">
+        <v>165</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>1</v>
+      </c>
+      <c r="O46" t="s">
+        <v>205</v>
+      </c>
+      <c r="P46" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>195</v>
+      </c>
+      <c r="D47" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" t="s">
+        <v>73</v>
+      </c>
+      <c r="F47" t="s">
+        <v>74</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="O47" t="s">
+        <v>205</v>
+      </c>
+      <c r="P47" s="1">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
+        <v>196</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
+        <v>115</v>
+      </c>
+      <c r="F48" t="s">
+        <v>203</v>
+      </c>
+      <c r="G48" t="s">
+        <v>204</v>
+      </c>
+      <c r="H48" t="s">
+        <v>169</v>
+      </c>
+      <c r="I48" t="s">
+        <v>170</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48" t="s">
+        <v>205</v>
+      </c>
+      <c r="P48" s="1">
+        <v>44055</v>
       </c>
     </row>
   </sheetData>

</xml_diff>